<commit_message>
read node location successfully
</commit_message>
<xml_diff>
--- a/dati_casoStudioItalia/network_data/capacities_distances.xlsx
+++ b/dati_casoStudioItalia/network_data/capacities_distances.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\DrinDrin\dati_casoStudioItalia\network_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E1D89EB7-DA92-4468-8132-79F6D01B978C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF377272-5341-47F6-B9C7-D324FC4BF5B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{91DA2F06-C22B-4D00-B2AC-01B40602F823}"/>
   </bookViews>
   <sheets>
-    <sheet name="Capacità di trasmissione MW" sheetId="2" r:id="rId1"/>
-    <sheet name="Distanza km" sheetId="1" r:id="rId2"/>
+    <sheet name="Info geografiche" sheetId="3" r:id="rId1"/>
+    <sheet name="Capacità di trasmissione MW" sheetId="2" r:id="rId2"/>
+    <sheet name="Distanza km" sheetId="1" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -59,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="10">
   <si>
     <t>IT-North</t>
   </si>
@@ -80,6 +81,15 @@
   </si>
   <si>
     <t>IT-Sardinia</t>
+  </si>
+  <si>
+    <t>latitude</t>
+  </si>
+  <si>
+    <t>longitude</t>
+  </si>
+  <si>
+    <t>altitude</t>
   </si>
 </sst>
 </file>
@@ -450,11 +460,75 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06FF2561-9D00-4F56-A261-A32E82066FE0}">
+  <dimension ref="A1:D8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="13.77734375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A491047D-1218-4647-9244-8974A4B6B6E2}">
   <dimension ref="A1:H8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J7" sqref="J7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -547,7 +621,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9DEAC826-F396-45BD-BD27-2D25F7438DDA}">
   <dimension ref="A1:H8"/>
   <sheetViews>

</xml_diff>

<commit_message>
Imported existing generation capacity
</commit_message>
<xml_diff>
--- a/dati_casoStudioItalia/network_data/capacities_distances.xlsx
+++ b/dati_casoStudioItalia/network_data/capacities_distances.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="600" firstSheet="3" activeTab="3" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="Info geografiche" sheetId="1" state="visible" r:id="rId1"/>
@@ -22,13 +22,18 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <color theme="1"/>
       <sz val="11"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Aptos Narrow"/>
+      <b val="1"/>
+      <sz val="11"/>
     </font>
     <font>
       <b val="1"/>
@@ -42,7 +47,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -124,6 +129,21 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin"/>
       <right style="thin"/>
       <top style="thin"/>
@@ -133,7 +153,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" pivotButton="0" quotePrefix="0" xfId="0"/>
@@ -143,6 +163,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
@@ -544,8 +567,8 @@
   </sheetPr>
   <dimension ref="A1:D8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
@@ -575,6 +598,15 @@
         <is>
           <t>NORD</t>
         </is>
+      </c>
+      <c r="B2" t="n">
+        <v>9999</v>
+      </c>
+      <c r="C2" t="n">
+        <v>9999</v>
+      </c>
+      <c r="D2" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="3">
@@ -639,44 +671,44 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="B1" s="8" t="inlineStr">
+      <c r="B1" s="9" t="inlineStr">
         <is>
           <t>NORD</t>
         </is>
       </c>
-      <c r="C1" s="8" t="inlineStr">
-        <is>
-          <t>CNOR</t>
-        </is>
-      </c>
-      <c r="D1" s="8" t="inlineStr">
-        <is>
-          <t>CSUD</t>
-        </is>
-      </c>
-      <c r="E1" s="8" t="inlineStr">
+      <c r="C1" s="9" t="inlineStr">
+        <is>
+          <t>CNOR</t>
+        </is>
+      </c>
+      <c r="D1" s="9" t="inlineStr">
+        <is>
+          <t>CSUD</t>
+        </is>
+      </c>
+      <c r="E1" s="9" t="inlineStr">
         <is>
           <t>SUD</t>
         </is>
       </c>
-      <c r="F1" s="8" t="inlineStr">
+      <c r="F1" s="9" t="inlineStr">
         <is>
           <t>CALA</t>
         </is>
       </c>
-      <c r="G1" s="8" t="inlineStr">
-        <is>
-          <t>SICI</t>
-        </is>
-      </c>
-      <c r="H1" s="8" t="inlineStr">
+      <c r="G1" s="9" t="inlineStr">
+        <is>
+          <t>SICI</t>
+        </is>
+      </c>
+      <c r="H1" s="9" t="inlineStr">
         <is>
           <t>SARD</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="8" t="inlineStr">
+      <c r="A2" s="9" t="inlineStr">
         <is>
           <t>NORD</t>
         </is>
@@ -704,7 +736,7 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="8" t="inlineStr">
+      <c r="A3" s="9" t="inlineStr">
         <is>
           <t>CNOR</t>
         </is>
@@ -732,7 +764,7 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="8" t="inlineStr">
+      <c r="A4" s="9" t="inlineStr">
         <is>
           <t>CSUD</t>
         </is>
@@ -760,7 +792,7 @@
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="8" t="inlineStr">
+      <c r="A5" s="9" t="inlineStr">
         <is>
           <t>SUD</t>
         </is>
@@ -788,7 +820,7 @@
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="8" t="inlineStr">
+      <c r="A6" s="9" t="inlineStr">
         <is>
           <t>CALA</t>
         </is>
@@ -816,7 +848,7 @@
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="8" t="inlineStr">
+      <c r="A7" s="9" t="inlineStr">
         <is>
           <t>SICI</t>
         </is>
@@ -844,7 +876,7 @@
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="8" t="inlineStr">
+      <c r="A8" s="9" t="inlineStr">
         <is>
           <t>SARD</t>
         </is>
@@ -872,20 +904,32 @@
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="8" t="inlineStr">
+      <c r="A9" s="9" t="inlineStr">
         <is>
           <t xml:space="preserve">SUD </t>
         </is>
       </c>
-      <c r="B9" t="inlineStr"/>
-      <c r="C9" t="inlineStr"/>
-      <c r="D9" t="inlineStr"/>
-      <c r="E9" t="inlineStr"/>
+      <c r="B9" t="n">
+        <v>0</v>
+      </c>
+      <c r="C9" t="n">
+        <v>0</v>
+      </c>
+      <c r="D9" t="n">
+        <v>0</v>
+      </c>
+      <c r="E9" t="n">
+        <v>0</v>
+      </c>
       <c r="F9" t="n">
         <v>1100</v>
       </c>
-      <c r="G9" t="inlineStr"/>
-      <c r="H9" t="inlineStr"/>
+      <c r="G9" t="n">
+        <v>0</v>
+      </c>
+      <c r="H9" t="n">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1028,7 +1072,7 @@
   </sheetPr>
   <dimension ref="A1:C15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A16" sqref="A16:D76"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Coded network except costs
</commit_message>
<xml_diff>
--- a/dati_casoStudioItalia/network_data/capacities_distances.xlsx
+++ b/dati_casoStudioItalia/network_data/capacities_distances.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="600" firstSheet="0" activeTab="2" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="Info geografiche" sheetId="1" state="visible" r:id="rId1"/>
@@ -15,7 +15,7 @@
     <sheet name="Raw data - tr. interna 2040" sheetId="7" state="visible" r:id="rId7"/>
   </sheets>
   <definedNames/>
-  <calcPr calcId="191029" fullCalcOnLoad="1"/>
+  <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -567,7 +567,7 @@
   </sheetPr>
   <dimension ref="A1:D8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
@@ -942,55 +942,58 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H8"/>
+  <dimension ref="A1:H9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
   <cols>
     <col width="13.77734375" bestFit="1" customWidth="1" min="1" max="1"/>
+    <col width="10" bestFit="1" customWidth="1" min="4" max="4"/>
+    <col width="11" bestFit="1" customWidth="1" min="5" max="5"/>
   </cols>
   <sheetData>
-    <row r="1" ht="15" customHeight="1" thickBot="1">
-      <c r="B1">
-        <f t="array" ref="B1:H1">TRANSPOSE(A2:A8)</f>
-        <v/>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>CNOR</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>CSUD</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
+    <row r="1" ht="15" customHeight="1">
+      <c r="B1" s="8" t="inlineStr">
+        <is>
+          <t>NORD</t>
+        </is>
+      </c>
+      <c r="C1" s="8" t="inlineStr">
+        <is>
+          <t>CNOR</t>
+        </is>
+      </c>
+      <c r="D1" s="8" t="inlineStr">
+        <is>
+          <t>CSUD</t>
+        </is>
+      </c>
+      <c r="E1" s="8" t="inlineStr">
         <is>
           <t>SUD</t>
         </is>
       </c>
-      <c r="F1" t="inlineStr">
+      <c r="F1" s="8" t="inlineStr">
         <is>
           <t>CALA</t>
         </is>
       </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>SICI</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
+      <c r="G1" s="8" t="inlineStr">
+        <is>
+          <t>SICI</t>
+        </is>
+      </c>
+      <c r="H1" s="8" t="inlineStr">
         <is>
           <t>SARD</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="1" t="inlineStr">
+      <c r="A2" s="8" t="inlineStr">
         <is>
           <t>NORD</t>
         </is>
@@ -998,9 +1001,15 @@
       <c r="B2" t="n">
         <v>0</v>
       </c>
+      <c r="C2" t="n">
+        <v>888888</v>
+      </c>
+      <c r="H2" t="n">
+        <v>444444</v>
+      </c>
     </row>
     <row r="3">
-      <c r="A3" s="2" t="inlineStr">
+      <c r="A3" s="8" t="inlineStr">
         <is>
           <t>CNOR</t>
         </is>
@@ -1010,7 +1019,7 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="2" t="inlineStr">
+      <c r="A4" s="8" t="inlineStr">
         <is>
           <t>CSUD</t>
         </is>
@@ -1020,7 +1029,7 @@
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="inlineStr">
+      <c r="A5" s="8" t="inlineStr">
         <is>
           <t>SUD</t>
         </is>
@@ -1030,7 +1039,7 @@
       </c>
     </row>
     <row r="6">
-      <c r="A6" t="inlineStr">
+      <c r="A6" s="8" t="inlineStr">
         <is>
           <t>CALA</t>
         </is>
@@ -1040,7 +1049,7 @@
       </c>
     </row>
     <row r="7">
-      <c r="A7" t="inlineStr">
+      <c r="A7" s="8" t="inlineStr">
         <is>
           <t>SICI</t>
         </is>
@@ -1048,15 +1057,25 @@
       <c r="G7" t="n">
         <v>0</v>
       </c>
+      <c r="H7" t="n">
+        <v>55555555</v>
+      </c>
     </row>
     <row r="8">
-      <c r="A8" t="inlineStr">
+      <c r="A8" s="8" t="inlineStr">
         <is>
           <t>SARD</t>
         </is>
       </c>
       <c r="H8" t="n">
         <v>0</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="8" t="inlineStr">
+        <is>
+          <t xml:space="preserve">SUD </t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>